<commit_message>
Rails: updates routes to be more strict about the format of buck ids
</commit_message>
<xml_diff>
--- a/lib/seed/users.xlsx
+++ b/lib/seed/users.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="754">
   <si>
     <t>Spot</t>
   </si>
@@ -2286,6 +2286,9 @@
   </si>
   <si>
     <t>peacock.1@fakeemail.com</t>
+  </si>
+  <si>
+    <t>Thompson-smith.1234</t>
   </si>
 </sst>
 </file>
@@ -2728,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="J117" sqref="J117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2929,7 +2932,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>24</v>
+        <v>753</v>
       </c>
       <c r="H6" t="s">
         <v>247</v>

</xml_diff>